<commit_message>
Edited test data, refactoring
</commit_message>
<xml_diff>
--- a/test-cases-manual/testCalc.xlsx
+++ b/test-cases-manual/testCalc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ataccama-test-task\test-cases-manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E86F161-24C1-46D1-BA2E-9A419F28AA6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A61285-039F-44BA-90BA-D83C3DDB4BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$C$90</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$C$88</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="8">
   <si>
     <t>addition</t>
   </si>
@@ -169,10 +169,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14290186-9F33-4F36-A60E-B08205E117B3}" name="out__3" displayName="out__3" ref="A1:D90" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D90" xr:uid="{CFD2BEAB-8E69-4A61-B802-1659BC867E32}"/>
-  <sortState ref="A2:C90">
-    <sortCondition ref="A1:A90"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14290186-9F33-4F36-A60E-B08205E117B3}" name="out__3" displayName="out__3" ref="A1:D88" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D88" xr:uid="{CFD2BEAB-8E69-4A61-B802-1659BC867E32}"/>
+  <sortState ref="A2:C88">
+    <sortCondition ref="A1:A88"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B125716F-F479-4092-9983-6B7BDB9EE6C6}" uniqueName="1" name="Operations" queryTableFieldId="1" dataDxfId="3"/>
@@ -449,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28051AC-C65F-40DA-9517-FDA463A27466}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +502,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D57" si="0">_xlfn.IFS(A3="addition",B3+C3,A3="subtraction",B3-C3,A3="division",B3/C3,A3="multiplication",B3*C3)</f>
+        <f t="shared" ref="D3:D55" si="0">_xlfn.IFS(A3="addition",B3+C3,A3="subtraction",B3-C3,A3="division",B3/C3,A3="multiplication",B3*C3)</f>
         <v>1</v>
       </c>
     </row>
@@ -1246,14 +1246,14 @@
         <v>2</v>
       </c>
       <c r="B53" s="2">
-        <v>215</v>
+        <v>-46340</v>
       </c>
       <c r="C53" s="2">
-        <v>2147483647</v>
+        <v>215</v>
       </c>
       <c r="D53" s="2">
         <f t="shared" si="0"/>
-        <v>461708984105</v>
+        <v>-9963100</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1261,14 +1261,14 @@
         <v>2</v>
       </c>
       <c r="B54" s="2">
-        <v>2147483647</v>
+        <v>0</v>
       </c>
       <c r="C54" s="2">
-        <v>215</v>
+        <v>15</v>
       </c>
       <c r="D54" s="2">
         <f t="shared" si="0"/>
-        <v>461708984105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1276,14 +1276,14 @@
         <v>2</v>
       </c>
       <c r="B55" s="2">
-        <v>-46340</v>
+        <v>15</v>
       </c>
       <c r="C55" s="2">
-        <v>215</v>
+        <v>1</v>
       </c>
       <c r="D55" s="2">
         <f t="shared" si="0"/>
-        <v>-9963100</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1291,14 +1291,14 @@
         <v>2</v>
       </c>
       <c r="B56" s="2">
-        <v>0</v>
+        <v>215</v>
       </c>
       <c r="C56" s="2">
-        <v>15</v>
+        <v>46341</v>
       </c>
       <c r="D56" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="D56:D88" si="1">_xlfn.IFS(A56="addition",B56+C56,A56="subtraction",B56-C56,A56="division",B56/C56,A56="multiplication",B56*C56)</f>
+        <v>9963315</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1309,11 +1309,11 @@
         <v>15</v>
       </c>
       <c r="C57" s="2">
-        <v>1</v>
+        <v>-2147483648</v>
       </c>
       <c r="D57" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f t="shared" si="1"/>
+        <v>-32212254720</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1321,14 +1321,14 @@
         <v>2</v>
       </c>
       <c r="B58" s="2">
-        <v>215</v>
+        <v>46341</v>
       </c>
       <c r="C58" s="2">
-        <v>46341</v>
+        <v>1</v>
       </c>
       <c r="D58" s="2">
-        <f t="shared" ref="D58:D90" si="1">_xlfn.IFS(A58="addition",B58+C58,A58="subtraction",B58-C58,A58="division",B58/C58,A58="multiplication",B58*C58)</f>
-        <v>9963315</v>
+        <f t="shared" si="1"/>
+        <v>46341</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1339,11 +1339,11 @@
         <v>15</v>
       </c>
       <c r="C59" s="2">
-        <v>-2147483648</v>
+        <v>-46340</v>
       </c>
       <c r="D59" s="2">
         <f t="shared" si="1"/>
-        <v>-32212254720</v>
+        <v>-695100</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1351,14 +1351,14 @@
         <v>2</v>
       </c>
       <c r="B60" s="2">
-        <v>46341</v>
+        <v>1</v>
       </c>
       <c r="C60" s="2">
-        <v>1</v>
+        <v>215</v>
       </c>
       <c r="D60" s="2">
         <f t="shared" si="1"/>
-        <v>46341</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1366,14 +1366,14 @@
         <v>2</v>
       </c>
       <c r="B61" s="2">
-        <v>15</v>
+        <v>46341</v>
       </c>
       <c r="C61" s="2">
-        <v>-46340</v>
+        <v>46341</v>
       </c>
       <c r="D61" s="2">
         <f t="shared" si="1"/>
-        <v>-695100</v>
+        <v>2147488281</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1384,11 +1384,11 @@
         <v>1</v>
       </c>
       <c r="C62" s="2">
-        <v>215</v>
+        <v>1</v>
       </c>
       <c r="D62" s="2">
         <f t="shared" si="1"/>
-        <v>215</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1396,44 +1396,44 @@
         <v>2</v>
       </c>
       <c r="B63" s="2">
-        <v>46341</v>
+        <v>-46340</v>
       </c>
       <c r="C63" s="2">
         <v>46341</v>
       </c>
       <c r="D63" s="2">
         <f t="shared" si="1"/>
-        <v>2147488281</v>
+        <v>-2147441940</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B64" s="2">
-        <v>1</v>
+        <v>215</v>
       </c>
       <c r="C64" s="2">
-        <v>1</v>
+        <v>46341</v>
       </c>
       <c r="D64" s="2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>-46126</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B65" s="2">
-        <v>-46340</v>
+        <v>0</v>
       </c>
       <c r="C65" s="2">
-        <v>46341</v>
+        <v>215</v>
       </c>
       <c r="D65" s="2">
         <f t="shared" si="1"/>
-        <v>-2147441940</v>
+        <v>-215</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1441,14 +1441,14 @@
         <v>1</v>
       </c>
       <c r="B66" s="2">
-        <v>215</v>
+        <v>15</v>
       </c>
       <c r="C66" s="2">
-        <v>46341</v>
+        <v>15</v>
       </c>
       <c r="D66" s="2">
         <f t="shared" si="1"/>
-        <v>-46126</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1456,14 +1456,14 @@
         <v>1</v>
       </c>
       <c r="B67" s="2">
-        <v>0</v>
+        <v>-46340</v>
       </c>
       <c r="C67" s="2">
-        <v>215</v>
+        <v>-46340</v>
       </c>
       <c r="D67" s="2">
         <f t="shared" si="1"/>
-        <v>-215</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1471,14 +1471,14 @@
         <v>1</v>
       </c>
       <c r="B68" s="2">
-        <v>15</v>
+        <v>2147483647</v>
       </c>
       <c r="C68" s="2">
-        <v>15</v>
+        <v>-2147483648</v>
       </c>
       <c r="D68" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4294967295</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1486,14 +1486,14 @@
         <v>1</v>
       </c>
       <c r="B69" s="2">
-        <v>-46340</v>
+        <v>-2147483648</v>
       </c>
       <c r="C69" s="2">
-        <v>-46340</v>
+        <v>0</v>
       </c>
       <c r="D69" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2147483648</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1501,14 +1501,14 @@
         <v>1</v>
       </c>
       <c r="B70" s="2">
-        <v>2147483647</v>
+        <v>0</v>
       </c>
       <c r="C70" s="2">
-        <v>-2147483648</v>
+        <v>1</v>
       </c>
       <c r="D70" s="2">
         <f t="shared" si="1"/>
-        <v>4294967295</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1516,14 +1516,14 @@
         <v>1</v>
       </c>
       <c r="B71" s="2">
+        <v>1</v>
+      </c>
+      <c r="C71" s="2">
         <v>-2147483648</v>
       </c>
-      <c r="C71" s="2">
-        <v>0</v>
-      </c>
       <c r="D71" s="2">
         <f t="shared" si="1"/>
-        <v>-2147483648</v>
+        <v>2147483649</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1531,14 +1531,14 @@
         <v>1</v>
       </c>
       <c r="B72" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C72" s="2">
         <v>1</v>
       </c>
       <c r="D72" s="2">
         <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1546,14 +1546,14 @@
         <v>1</v>
       </c>
       <c r="B73" s="2">
-        <v>1</v>
+        <v>215</v>
       </c>
       <c r="C73" s="2">
-        <v>-2147483648</v>
+        <v>215</v>
       </c>
       <c r="D73" s="2">
         <f t="shared" si="1"/>
-        <v>2147483649</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1561,14 +1561,14 @@
         <v>1</v>
       </c>
       <c r="B74" s="2">
-        <v>15</v>
+        <v>2147483647</v>
       </c>
       <c r="C74" s="2">
-        <v>1</v>
+        <v>46341</v>
       </c>
       <c r="D74" s="2">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>2147437306</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1576,10 +1576,10 @@
         <v>1</v>
       </c>
       <c r="B75" s="2">
-        <v>215</v>
+        <v>1</v>
       </c>
       <c r="C75" s="2">
-        <v>215</v>
+        <v>1</v>
       </c>
       <c r="D75" s="2">
         <f t="shared" si="1"/>
@@ -1591,14 +1591,14 @@
         <v>1</v>
       </c>
       <c r="B76" s="2">
-        <v>2147483647</v>
+        <v>46341</v>
       </c>
       <c r="C76" s="2">
-        <v>46341</v>
+        <v>215</v>
       </c>
       <c r="D76" s="2">
         <f t="shared" si="1"/>
-        <v>2147437306</v>
+        <v>46126</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -1606,14 +1606,14 @@
         <v>1</v>
       </c>
       <c r="B77" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C77" s="2">
-        <v>1</v>
+        <v>2147483647</v>
       </c>
       <c r="D77" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2147483632</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1621,14 +1621,14 @@
         <v>1</v>
       </c>
       <c r="B78" s="2">
-        <v>46341</v>
+        <v>215</v>
       </c>
       <c r="C78" s="2">
-        <v>215</v>
+        <v>1</v>
       </c>
       <c r="D78" s="2">
         <f t="shared" si="1"/>
-        <v>46126</v>
+        <v>214</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1636,14 +1636,14 @@
         <v>1</v>
       </c>
       <c r="B79" s="2">
-        <v>15</v>
+        <v>2147483647</v>
       </c>
       <c r="C79" s="2">
-        <v>2147483647</v>
+        <v>15</v>
       </c>
       <c r="D79" s="2">
         <f t="shared" si="1"/>
-        <v>-2147483632</v>
+        <v>2147483632</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1651,14 +1651,14 @@
         <v>1</v>
       </c>
       <c r="B80" s="2">
-        <v>215</v>
+        <v>1</v>
       </c>
       <c r="C80" s="2">
-        <v>1</v>
+        <v>2147483647</v>
       </c>
       <c r="D80" s="2">
         <f t="shared" si="1"/>
-        <v>214</v>
+        <v>-2147483646</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1666,14 +1666,14 @@
         <v>1</v>
       </c>
       <c r="B81" s="2">
-        <v>2147483647</v>
+        <v>-2147483648</v>
       </c>
       <c r="C81" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D81" s="2">
         <f t="shared" si="1"/>
-        <v>2147483632</v>
+        <v>-2147483649</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1681,14 +1681,14 @@
         <v>1</v>
       </c>
       <c r="B82" s="2">
-        <v>1</v>
+        <v>-2147483648</v>
       </c>
       <c r="C82" s="2">
         <v>2147483647</v>
       </c>
       <c r="D82" s="2">
         <f t="shared" si="1"/>
-        <v>-2147483646</v>
+        <v>-4294967295</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1696,14 +1696,14 @@
         <v>1</v>
       </c>
       <c r="B83" s="2">
-        <v>-2147483648</v>
+        <v>0</v>
       </c>
       <c r="C83" s="2">
-        <v>1</v>
+        <v>46341</v>
       </c>
       <c r="D83" s="2">
         <f t="shared" si="1"/>
-        <v>-2147483649</v>
+        <v>-46341</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -1711,14 +1711,14 @@
         <v>1</v>
       </c>
       <c r="B84" s="2">
-        <v>-2147483648</v>
+        <v>15</v>
       </c>
       <c r="C84" s="2">
-        <v>2147483647</v>
+        <v>0</v>
       </c>
       <c r="D84" s="2">
         <f t="shared" si="1"/>
-        <v>-4294967295</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -1726,14 +1726,14 @@
         <v>1</v>
       </c>
       <c r="B85" s="2">
-        <v>0</v>
+        <v>2147483647</v>
       </c>
       <c r="C85" s="2">
-        <v>46341</v>
+        <v>0</v>
       </c>
       <c r="D85" s="2">
         <f t="shared" si="1"/>
-        <v>-46341</v>
+        <v>2147483647</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1741,14 +1741,14 @@
         <v>1</v>
       </c>
       <c r="B86" s="2">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C86" s="2">
-        <v>0</v>
+        <v>46341</v>
       </c>
       <c r="D86" s="2">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>-46340</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -1756,14 +1756,14 @@
         <v>1</v>
       </c>
       <c r="B87" s="2">
-        <v>2147483647</v>
+        <v>215</v>
       </c>
       <c r="C87" s="2">
-        <v>0</v>
+        <v>-46340</v>
       </c>
       <c r="D87" s="2">
         <f t="shared" si="1"/>
-        <v>2147483647</v>
+        <v>46555</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -1771,42 +1771,12 @@
         <v>1</v>
       </c>
       <c r="B88" s="2">
-        <v>1</v>
+        <v>-2147483648</v>
       </c>
       <c r="C88" s="2">
         <v>46341</v>
       </c>
       <c r="D88" s="2">
-        <f t="shared" si="1"/>
-        <v>-46340</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B89" s="2">
-        <v>215</v>
-      </c>
-      <c r="C89" s="2">
-        <v>-46340</v>
-      </c>
-      <c r="D89" s="2">
-        <f t="shared" si="1"/>
-        <v>46555</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B90" s="2">
-        <v>-2147483648</v>
-      </c>
-      <c r="C90" s="2">
-        <v>46341</v>
-      </c>
-      <c r="D90" s="2">
         <f t="shared" si="1"/>
         <v>-2147529989</v>
       </c>

</xml_diff>